<commit_message>
non mi ricordo nono era la cosa del era la cosa del nono non scrivere un commit serio
</commit_message>
<xml_diff>
--- a/data_lab1_FINALE.xlsx
+++ b/data_lab1_FINALE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Calibrazione" sheetId="1" state="visible" r:id="rId3"/>
@@ -1209,11 +1209,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="86169146"/>
-        <c:axId val="75196289"/>
+        <c:axId val="5699997"/>
+        <c:axId val="97926599"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86169146"/>
+        <c:axId val="5699997"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1255,12 +1255,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75196289"/>
+        <c:crossAx val="97926599"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75196289"/>
+        <c:axId val="97926599"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1302,7 +1302,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86169146"/>
+        <c:crossAx val="5699997"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1544,7 +1544,7 @@
   </sheetPr>
   <dimension ref="A1:U88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B3" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B3" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -3991,8 +3991,8 @@
   </sheetPr>
   <dimension ref="B3:XFD107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I45" activeCellId="0" sqref="I45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G102" activeCellId="0" sqref="G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6502,7 +6502,7 @@
         <v>29.0043100245464</v>
       </c>
       <c r="F104" s="2" t="n">
-        <v>0.039</v>
+        <v>0.04</v>
       </c>
       <c r="H104" s="1" t="n">
         <v>4.77</v>
@@ -6530,7 +6530,7 @@
         <v>29.4416371827383</v>
       </c>
       <c r="F105" s="2" t="n">
-        <v>0.046</v>
+        <v>0.05</v>
       </c>
       <c r="H105" s="1" t="n">
         <v>6.42</v>
@@ -6558,7 +6558,7 @@
         <v>29.8846114246112</v>
       </c>
       <c r="F106" s="2" t="n">
-        <v>0.051</v>
+        <v>0.05</v>
       </c>
       <c r="H106" s="1" t="n">
         <v>7.85</v>
@@ -6586,7 +6586,7 @@
         <v>30.3329853459893</v>
       </c>
       <c r="F107" s="2" t="n">
-        <v>0.059</v>
+        <v>0.06</v>
       </c>
       <c r="H107" s="1" t="n">
         <v>9.75</v>
@@ -6624,8 +6624,8 @@
   </sheetPr>
   <dimension ref="B2:K145"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K75" activeCellId="0" sqref="K75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I69" activeCellId="0" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8935,7 +8935,7 @@
         <v>1.5337861650178</v>
       </c>
       <c r="F83" s="2" t="n">
-        <v>0.002004</v>
+        <v>0.002</v>
       </c>
       <c r="G83" s="2"/>
       <c r="H83" s="25"/>
@@ -8952,7 +8952,7 @@
         <v>1.75285481429581</v>
       </c>
       <c r="F84" s="2" t="n">
-        <v>0.002008</v>
+        <v>0.002</v>
       </c>
       <c r="G84" s="2"/>
       <c r="H84" s="25"/>
@@ -8969,7 +8969,7 @@
         <v>1.96834956245074</v>
       </c>
       <c r="F85" s="2" t="n">
-        <v>0.002012</v>
+        <v>0.002</v>
       </c>
       <c r="G85" s="2"/>
       <c r="H85" s="25"/>
@@ -8986,7 +8986,7 @@
         <v>2.09353767580142</v>
       </c>
       <c r="F86" s="2" t="n">
-        <v>0.002016</v>
+        <v>0.002</v>
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="25"/>
@@ -9003,7 +9003,7 @@
         <v>2.2477766792989</v>
       </c>
       <c r="F87" s="2" t="n">
-        <v>0.00202</v>
+        <v>0.002</v>
       </c>
       <c r="G87" s="2"/>
       <c r="H87" s="25"/>
@@ -9020,7 +9020,7 @@
         <v>2.94278779391243</v>
       </c>
       <c r="F88" s="2" t="n">
-        <v>0.002024</v>
+        <v>0.002</v>
       </c>
       <c r="G88" s="2"/>
       <c r="H88" s="25"/>
@@ -9037,7 +9037,7 @@
         <v>2.9859001992699</v>
       </c>
       <c r="F89" s="2" t="n">
-        <v>0.002028</v>
+        <v>0.002</v>
       </c>
       <c r="G89" s="2"/>
       <c r="H89" s="25"/>
@@ -9054,7 +9054,7 @@
         <v>3.07382497875204</v>
       </c>
       <c r="F90" s="2" t="n">
-        <v>0.002032</v>
+        <v>0.002</v>
       </c>
       <c r="G90" s="2"/>
       <c r="H90" s="25"/>
@@ -9071,7 +9071,7 @@
         <v>3.16385840391128</v>
       </c>
       <c r="F91" s="2" t="n">
-        <v>0.002036</v>
+        <v>0.002</v>
       </c>
       <c r="G91" s="2"/>
       <c r="H91" s="25"/>
@@ -9088,7 +9088,7 @@
         <v>3.25582554815211</v>
       </c>
       <c r="F92" s="2" t="n">
-        <v>0.002044</v>
+        <v>0.002</v>
       </c>
       <c r="G92" s="2"/>
       <c r="H92" s="25"/>
@@ -9105,7 +9105,7 @@
         <v>3.34956713621328</v>
       </c>
       <c r="F93" s="2" t="n">
-        <v>0.002048</v>
+        <v>0.002</v>
       </c>
       <c r="G93" s="2"/>
       <c r="H93" s="25"/>
@@ -9122,7 +9122,7 @@
         <v>3.44493831584834</v>
       </c>
       <c r="F94" s="2" t="n">
-        <v>0.002056</v>
+        <v>0.002</v>
       </c>
       <c r="G94" s="2"/>
       <c r="H94" s="25"/>
@@ -9139,7 +9139,7 @@
         <v>3.54180744818235</v>
       </c>
       <c r="F95" s="1" t="n">
-        <v>0.002064</v>
+        <v>0.002</v>
       </c>
       <c r="I95" s="22"/>
     </row>
@@ -9154,7 +9154,7 @@
         <v>3.64005494464026</v>
       </c>
       <c r="F96" s="1" t="n">
-        <v>0.002072</v>
+        <v>0.002</v>
       </c>
       <c r="I96" s="22"/>
     </row>
@@ -9169,7 +9169,7 @@
         <v>3.73957216804276</v>
       </c>
       <c r="F97" s="1" t="n">
-        <v>0.00208</v>
+        <v>0.002</v>
       </c>
       <c r="I97" s="22"/>
     </row>
@@ -9184,7 +9184,7 @@
         <v>3.84026040783695</v>
       </c>
       <c r="F98" s="1" t="n">
-        <v>0.002092</v>
+        <v>0.002</v>
       </c>
       <c r="I98" s="22"/>
     </row>
@@ -9199,7 +9199,7 @@
         <v>3.94202993392998</v>
       </c>
       <c r="F99" s="1" t="n">
-        <v>0.002108</v>
+        <v>0.002</v>
       </c>
       <c r="I99" s="22"/>
     </row>
@@ -9214,7 +9214,7 @@
         <v>4.04479912974674</v>
       </c>
       <c r="F100" s="1" t="n">
-        <v>0.00212</v>
+        <v>0.002</v>
       </c>
       <c r="I100" s="22"/>
     </row>
@@ -9229,7 +9229,7 @@
         <v>4.14849370253831</v>
       </c>
       <c r="F101" s="1" t="n">
-        <v>0.002136</v>
+        <v>0.002</v>
       </c>
       <c r="I101" s="22"/>
     </row>
@@ -9244,7 +9244,7 @@
         <v>4.2530459673039</v>
       </c>
       <c r="F102" s="1" t="n">
-        <v>0.002156</v>
+        <v>0.002</v>
       </c>
       <c r="I102" s="22"/>
     </row>
@@ -9259,7 +9259,7 @@
         <v>4.35839419970245</v>
       </c>
       <c r="F103" s="1" t="n">
-        <v>0.002172</v>
+        <v>0.002</v>
       </c>
       <c r="I103" s="22"/>
     </row>
@@ -9274,7 +9274,7 @@
         <v>6.3608175575157</v>
       </c>
       <c r="F104" s="1" t="n">
-        <v>0.00218</v>
+        <v>0.002</v>
       </c>
       <c r="I104" s="22"/>
     </row>
@@ -9289,7 +9289,7 @@
         <v>6.45387480510739</v>
       </c>
       <c r="F105" s="1" t="n">
-        <v>0.002212</v>
+        <v>0.002</v>
       </c>
       <c r="I105" s="22"/>
     </row>
@@ -9304,7 +9304,7 @@
         <v>6.54904573201318</v>
       </c>
       <c r="F106" s="1" t="n">
-        <v>0.002232</v>
+        <v>0.002</v>
       </c>
       <c r="I106" s="22"/>
     </row>
@@ -9319,7 +9319,7 @@
         <v>6.64623953826523</v>
       </c>
       <c r="F107" s="1" t="n">
-        <v>0.002268</v>
+        <v>0.002</v>
       </c>
       <c r="I107" s="22"/>
     </row>
@@ -9334,7 +9334,7 @@
         <v>6.74536878161602</v>
       </c>
       <c r="F108" s="1" t="n">
-        <v>0.002312</v>
+        <v>0.002</v>
       </c>
       <c r="I108" s="22"/>
     </row>
@@ -9349,7 +9349,7 @@
         <v>6.84634939219435</v>
       </c>
       <c r="F109" s="1" t="n">
-        <v>0.002352</v>
+        <v>0.002</v>
       </c>
       <c r="I109" s="22"/>
     </row>
@@ -9364,7 +9364,7 @@
         <v>6.94910066123668</v>
       </c>
       <c r="F110" s="1" t="n">
-        <v>0.0024</v>
+        <v>0.002</v>
       </c>
       <c r="I110" s="22"/>
     </row>
@@ -9379,7 +9379,7 @@
         <v>7.05354520790786</v>
       </c>
       <c r="F111" s="1" t="n">
-        <v>0.002456</v>
+        <v>0.002</v>
       </c>
       <c r="I111" s="22"/>
     </row>
@@ -9394,7 +9394,7 @@
         <v>7.1596089278675</v>
       </c>
       <c r="F112" s="1" t="n">
-        <v>0.00252</v>
+        <v>0.003</v>
       </c>
       <c r="I112" s="22"/>
     </row>
@@ -9409,7 +9409,7 @@
         <v>7.26722092687432</v>
       </c>
       <c r="F113" s="1" t="n">
-        <v>0.002576</v>
+        <v>0.003</v>
       </c>
       <c r="I113" s="22"/>
     </row>
@@ -9424,7 +9424,7 @@
         <v>7.37631344236401</v>
       </c>
       <c r="F114" s="1" t="n">
-        <v>0.002656</v>
+        <v>0.003</v>
       </c>
       <c r="I114" s="22"/>
     </row>
@@ -9439,7 +9439,7 @@
         <v>7.48682175559162</v>
       </c>
       <c r="F115" s="1" t="n">
-        <v>0.002736</v>
+        <v>0.003</v>
       </c>
       <c r="I115" s="22"/>
     </row>
@@ -9454,7 +9454,7 @@
         <v>7.59868409660515</v>
       </c>
       <c r="F116" s="1" t="n">
-        <v>0.002816</v>
+        <v>0.003</v>
       </c>
       <c r="I116" s="22"/>
     </row>
@@ -9469,7 +9469,7 @@
         <v>7.71184154401528</v>
       </c>
       <c r="F117" s="1" t="n">
-        <v>0.002932</v>
+        <v>0.003</v>
       </c>
       <c r="I117" s="22"/>
     </row>
@@ -9484,7 +9484,7 @@
         <v>7.82623792124926</v>
       </c>
       <c r="F118" s="1" t="n">
-        <v>0.002996</v>
+        <v>0.003</v>
       </c>
       <c r="I118" s="22"/>
     </row>
@@ -9499,7 +9499,7 @@
         <v>7.9418196907258</v>
       </c>
       <c r="F119" s="1" t="n">
-        <v>0.00312</v>
+        <v>0.003</v>
       </c>
       <c r="I119" s="22"/>
     </row>
@@ -9514,7 +9514,7 @@
         <v>8.05853584716231</v>
       </c>
       <c r="F120" s="1" t="n">
-        <v>0.003264</v>
+        <v>0.003</v>
       </c>
       <c r="I120" s="22"/>
     </row>
@@ -9529,7 +9529,7 @@
         <v>8.17633781102518</v>
       </c>
       <c r="F121" s="1" t="n">
-        <v>0.003404</v>
+        <v>0.003</v>
       </c>
       <c r="I121" s="22"/>
     </row>
@@ -9544,7 +9544,7 @@
         <v>8.2951793229562</v>
       </c>
       <c r="F122" s="1" t="n">
-        <v>0.00356</v>
+        <v>0.004</v>
       </c>
       <c r="I122" s="22"/>
     </row>
@@ -9559,7 +9559,7 @@
         <v>8.41501633985342</v>
       </c>
       <c r="F123" s="1" t="n">
-        <v>0.003712</v>
+        <v>0.004</v>
       </c>
       <c r="I123" s="22"/>
     </row>
@@ -9574,7 +9574,7 @@
         <v>8.53580693314932</v>
       </c>
       <c r="F124" s="1" t="n">
-        <v>0.00392</v>
+        <v>0.004</v>
       </c>
       <c r="I124" s="22"/>
     </row>
@@ -9589,7 +9589,7 @@
         <v>8.65751118971267</v>
       </c>
       <c r="F125" s="1" t="n">
-        <v>0.004136</v>
+        <v>0.004</v>
       </c>
       <c r="I125" s="22"/>
     </row>
@@ -9604,7 +9604,7 @@
         <v>8.78009111570034</v>
       </c>
       <c r="F126" s="1" t="n">
-        <v>0.004364</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9618,7 +9618,7 @@
         <v>8.9035105436002</v>
       </c>
       <c r="F127" s="1" t="n">
-        <v>0.00458</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9632,7 +9632,7 @@
         <v>9.02773504263389</v>
       </c>
       <c r="F128" s="1" t="n">
-        <v>0.00488</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9646,7 +9646,7 @@
         <v>9.1527318326279</v>
       </c>
       <c r="F129" s="1" t="n">
-        <v>0.005212</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9660,7 +9660,7 @@
         <v>9.2784697014109</v>
       </c>
       <c r="F130" s="1" t="n">
-        <v>0.005532</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9674,7 +9674,7 @@
         <v>9.40491892575369</v>
       </c>
       <c r="F131" s="1" t="n">
-        <v>0.0059</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9688,7 +9688,7 @@
         <v>9.53205119583398</v>
       </c>
       <c r="F132" s="1" t="n">
-        <v>0.006328</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9702,7 +9702,7 @@
         <v>9.65983954318083</v>
       </c>
       <c r="F133" s="1" t="n">
-        <v>0.006788</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9716,7 +9716,7 @@
         <v>9.78825827203185</v>
       </c>
       <c r="F134" s="1" t="n">
-        <v>0.007264</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9730,7 +9730,7 @@
         <v>9.91728289401891</v>
       </c>
       <c r="F135" s="1" t="n">
-        <v>0.00774</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9744,7 +9744,7 @@
         <v>10.0468900660851</v>
       </c>
       <c r="F136" s="1" t="n">
-        <v>0.008432</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9758,7 +9758,7 @@
         <v>10.1770575315265</v>
       </c>
       <c r="F137" s="1" t="n">
-        <v>0.008948</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9772,7 +9772,7 @@
         <v>10.3077640640442</v>
       </c>
       <c r="F138" s="1" t="n">
-        <v>0.00974</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9786,7 +9786,7 @@
         <v>10.4389894146895</v>
       </c>
       <c r="F139" s="1" t="n">
-        <v>0.01038</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9800,7 +9800,7 @@
         <v>10.5707142615814</v>
       </c>
       <c r="F140" s="1" t="n">
-        <v>0.011264</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9814,7 +9814,7 @@
         <v>10.7029201622735</v>
       </c>
       <c r="F141" s="1" t="n">
-        <v>0.012044</v>
+        <v>0.012</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9828,7 +9828,7 @@
         <v>10.8355895086516</v>
       </c>
       <c r="F142" s="1" t="n">
-        <v>0.013064</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9856,7 +9856,7 @@
         <v>11.1022520238013</v>
       </c>
       <c r="F144" s="1" t="n">
-        <v>0.015024</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9870,7 +9870,7 @@
         <v>14.293005282305</v>
       </c>
       <c r="F145" s="1" t="n">
-        <v>0.017232</v>
+        <v>0.017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>